<commit_message>
created multipage app to show official guide alongside ml model
</commit_message>
<xml_diff>
--- a/Tuning Database.xlsx
+++ b/Tuning Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackrockett/PycharmProjects/J70_Tuning_Guide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2511F8D6-C7C3-EA45-8E1C-BFFE52005B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D26ED01-D327-CA4F-AAD5-03364062A75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="50">
   <si>
     <t>RAKE</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>CREW_WEIGHT</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-1</t>
   </si>
 </sst>
 </file>
@@ -172,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -182,6 +191,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1006,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBEFC84-B3D8-FE4A-AFC9-8F9DD284FE98}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1051,8 +1066,8 @@
       <c r="C2" s="2">
         <v>-2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
+      <c r="D2" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E2" s="2">
         <v>15</v>
@@ -1080,8 +1095,8 @@
       <c r="C3" s="2">
         <v>-2</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E3" s="2">
         <v>15</v>
@@ -1109,8 +1124,8 @@
       <c r="C4" s="2">
         <v>-2</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
+      <c r="D4" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E4" s="2">
         <v>15</v>
@@ -1138,8 +1153,8 @@
       <c r="C5" s="2">
         <v>-2</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
+      <c r="D5" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E5" s="2">
         <v>15</v>
@@ -1167,8 +1182,8 @@
       <c r="C6" s="2">
         <v>-2</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
+      <c r="D6" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E6" s="2">
         <v>15</v>
@@ -1196,8 +1211,8 @@
       <c r="C7" s="2">
         <v>-1</v>
       </c>
-      <c r="D7" s="2">
-        <v>-1</v>
+      <c r="D7" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E7" s="2">
         <v>17</v>
@@ -1225,8 +1240,8 @@
       <c r="C8" s="2">
         <v>-1</v>
       </c>
-      <c r="D8" s="2">
-        <v>-1</v>
+      <c r="D8" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E8" s="2">
         <v>17</v>
@@ -1252,10 +1267,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2">
         <v>19</v>
@@ -1281,10 +1296,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2">
         <v>19</v>
@@ -1310,10 +1325,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2">
         <v>19</v>
@@ -1632,7 +1647,7 @@
         <v>-2</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E22" s="6">
         <v>15</v>
@@ -1661,7 +1676,7 @@
         <v>-2</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E23" s="6">
         <v>15</v>
@@ -1690,7 +1705,7 @@
         <v>-2</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E24" s="6">
         <v>15</v>
@@ -1719,7 +1734,7 @@
         <v>-2</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E25" s="6">
         <v>15</v>
@@ -1748,7 +1763,7 @@
         <v>-2</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E26" s="6">
         <v>15</v>
@@ -1777,7 +1792,7 @@
         <v>-2</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E27" s="6">
         <v>15</v>
@@ -1806,7 +1821,7 @@
         <v>-2</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E28" s="6">
         <v>15</v>
@@ -1890,10 +1905,10 @@
         <v>10</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E31" s="6">
         <v>19</v>
@@ -1919,10 +1934,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E32" s="6">
         <v>19</v>
@@ -1948,10 +1963,10 @@
         <v>12</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E33" s="6">
         <v>19</v>
@@ -2202,6 +2217,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
removed indexing of pandas df
</commit_message>
<xml_diff>
--- a/Tuning Database.xlsx
+++ b/Tuning Database.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackrockett/PycharmProjects/J70_Tuning_Guide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D26ED01-D327-CA4F-AAD5-03364062A75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB3A166-91CF-8C45-AA4C-D72F7FADCB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rig Tuning Database" sheetId="1" r:id="rId1"/>
     <sheet name="Rig_by_weight" sheetId="3" r:id="rId2"/>
     <sheet name="JIB Tuning Database" sheetId="2" r:id="rId3"/>
+    <sheet name="Template" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="50">
   <si>
     <t>RAKE</t>
   </si>
@@ -181,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -191,6 +192,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -228,12 +236,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -457,8 +466,8 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1021,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBEFC84-B3D8-FE4A-AFC9-8F9DD284FE98}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1066,7 +1075,7 @@
       <c r="C2" s="2">
         <v>-2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="2">
@@ -1095,7 +1104,7 @@
       <c r="C3" s="2">
         <v>-2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="2">
@@ -1124,7 +1133,7 @@
       <c r="C4" s="2">
         <v>-2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E4" s="2">
@@ -1153,7 +1162,7 @@
       <c r="C5" s="2">
         <v>-2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E5" s="2">
@@ -1182,7 +1191,7 @@
       <c r="C6" s="2">
         <v>-2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="2">
@@ -1211,7 +1220,7 @@
       <c r="C7" s="2">
         <v>-1</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="2">
@@ -1240,7 +1249,7 @@
       <c r="C8" s="2">
         <v>-1</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="2">
@@ -1637,587 +1646,587 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A22" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B22" s="6">
+      <c r="A22" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B22" s="7">
         <v>1</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="7">
         <v>-2</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="7">
         <v>15</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="F22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="7">
         <v>0</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A23" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B23" s="6">
+      <c r="A23" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B23" s="7">
         <v>2</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="7">
         <v>-2</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="7">
         <v>15</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="F23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="7">
         <v>0</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A24" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B24" s="6">
+      <c r="A24" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B24" s="7">
         <v>3</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="7">
         <v>-2</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="7">
         <v>15</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="6" t="s">
+      <c r="F24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="7">
         <v>0</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A25" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B25" s="6">
+      <c r="A25" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B25" s="7">
         <v>4</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="7">
         <v>-2</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="7">
         <v>15</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="F25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="7">
         <v>0</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A26" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B26" s="6">
+      <c r="A26" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B26" s="7">
         <v>5</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="7">
         <v>-2</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="7">
         <v>15</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="6" t="s">
+      <c r="F26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="7">
         <v>0</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A27" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B27" s="6">
+      <c r="A27" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B27" s="7">
         <v>6</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="7">
         <v>-2</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="7">
         <v>15</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="6" t="s">
+      <c r="F27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="7">
         <v>0</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A28" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B28" s="6">
+      <c r="A28" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B28" s="7">
         <v>7</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="7">
         <v>-2</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="7">
         <v>15</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="6" t="s">
+      <c r="F28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="7">
         <v>0</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A29" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B29" s="6">
+      <c r="A29" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B29" s="7">
         <v>8</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="7">
         <v>-1</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="7">
         <v>-1</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="7">
         <v>17</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="6" t="s">
+      <c r="F29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A30" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B30" s="6">
-        <v>9</v>
-      </c>
-      <c r="C30" s="6">
+      <c r="A30" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B30" s="7">
+        <v>9</v>
+      </c>
+      <c r="C30" s="7">
         <v>-1</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="7">
         <v>-1</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="7">
         <v>17</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="6" t="s">
+      <c r="F30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A31" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B31" s="6">
+      <c r="A31" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B31" s="7">
         <v>10</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="7">
         <v>19</v>
       </c>
-      <c r="F31" s="6">
-        <v>9</v>
-      </c>
-      <c r="G31" s="6" t="s">
+      <c r="F31" s="7">
+        <v>9</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A32" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B32" s="6">
+      <c r="A32" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B32" s="7">
         <v>11</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="7">
         <v>19</v>
       </c>
-      <c r="F32" s="6">
-        <v>9</v>
-      </c>
-      <c r="G32" s="6" t="s">
+      <c r="F32" s="7">
+        <v>9</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A33" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B33" s="6">
+      <c r="A33" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B33" s="7">
         <v>12</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="7">
         <v>19</v>
       </c>
-      <c r="F33" s="6">
-        <v>9</v>
-      </c>
-      <c r="G33" s="6" t="s">
+      <c r="F33" s="7">
+        <v>9</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A34" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B34" s="6">
+      <c r="A34" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B34" s="7">
         <v>13</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="7">
         <v>2</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="7">
         <v>2</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="7">
         <v>21</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="7">
         <v>13</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A35" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B35" s="6">
+      <c r="A35" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B35" s="7">
         <v>14</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="7">
         <v>2</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="7">
         <v>2</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="7">
         <v>21</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="7">
         <v>13</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A36" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B36" s="6">
+      <c r="A36" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B36" s="7">
         <v>15</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="7">
         <v>3</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="7">
         <v>3</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="7">
         <v>23</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="7">
         <v>16</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A37" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B37" s="6">
+      <c r="A37" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B37" s="7">
         <v>16</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="7">
         <v>4</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="7">
         <v>4</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="7">
         <v>24</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="7">
         <v>21</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I37" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A38" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B38" s="6">
+      <c r="A38" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B38" s="7">
         <v>17</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="7">
         <v>5</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="7">
         <v>5</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="7">
         <v>26</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="7">
         <v>23</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H38" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A39" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B39" s="6">
+      <c r="A39" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B39" s="7">
         <v>18</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="7">
         <v>6</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="7">
         <v>6</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="7">
         <v>27</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="7">
         <v>27</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G39" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H39" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I39" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A40" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B40" s="6">
+      <c r="A40" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B40" s="7">
         <v>19</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="7">
         <v>7</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="7">
         <v>7</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="7">
         <v>28</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="7">
         <v>28</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G40" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="7">
         <v>1</v>
       </c>
-      <c r="I40" s="7">
+      <c r="I40" s="8">
         <v>440</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A41" s="5">
-        <v>1425</v>
-      </c>
-      <c r="B41" s="6">
+      <c r="A41" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B41" s="7">
         <v>20</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="7">
         <v>7</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="7">
         <v>7</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="7">
         <v>28</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="7">
         <v>28</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="7">
         <v>1</v>
       </c>
-      <c r="I41" s="7">
+      <c r="I41" s="8">
         <v>440</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3061,4 +3070,196 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E34554-567E-4640-BB10-BF8C510B0742}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating to Twiggy Spec
</commit_message>
<xml_diff>
--- a/Tuning Database.xlsx
+++ b/Tuning Database.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajackrockett/PycharmProjects/J70_Tuning_Guide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8BC3C7-E2E8-E243-8C37-CEC0FF7B14B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF872D5-168C-0541-A862-C588357EB29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rig Tuning Database" sheetId="1" r:id="rId1"/>
-    <sheet name="Rig_by_weight" sheetId="3" r:id="rId2"/>
-    <sheet name="JIB Tuning Database" sheetId="2" r:id="rId3"/>
-    <sheet name="Template" sheetId="5" r:id="rId4"/>
-    <sheet name="Polars" sheetId="6" r:id="rId5"/>
+    <sheet name="JIB Tuning Database" sheetId="2" r:id="rId2"/>
+    <sheet name="Template" sheetId="5" r:id="rId3"/>
+    <sheet name="Polars" sheetId="6" r:id="rId4"/>
+    <sheet name="Rig_by_weight" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="68">
   <si>
     <t>RAKE</t>
   </si>
@@ -205,6 +205,42 @@
   </si>
   <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -1461,16 +1497,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>89123</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>133685</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>479035</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>155965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>475693</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>23618</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>41220</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>45898</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1702,7 +1738,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2003,14 +2039,14 @@
       <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2">
-        <v>21</v>
+      <c r="C12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="F12" s="2">
         <v>13</v>
@@ -2032,8 +2068,8 @@
       <c r="C13" s="2">
         <v>2</v>
       </c>
-      <c r="D13" s="2">
-        <v>2</v>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="E13" s="2">
         <v>21</v>
@@ -2058,8 +2094,8 @@
       <c r="C14" s="2">
         <v>3</v>
       </c>
-      <c r="D14" s="2">
-        <v>3</v>
+      <c r="D14" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="E14" s="2">
         <v>23</v>
@@ -2084,8 +2120,8 @@
       <c r="C15" s="2">
         <v>4</v>
       </c>
-      <c r="D15" s="2">
-        <v>4</v>
+      <c r="D15" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="E15" s="2">
         <v>24</v>
@@ -2110,8 +2146,8 @@
       <c r="C16" s="2">
         <v>5</v>
       </c>
-      <c r="D16" s="2">
-        <v>5</v>
+      <c r="D16" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E16" s="2">
         <v>26</v>
@@ -2136,8 +2172,8 @@
       <c r="C17" s="2">
         <v>6</v>
       </c>
-      <c r="D17" s="2">
-        <v>6</v>
+      <c r="D17" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="E17" s="2">
         <v>27</v>
@@ -2162,8 +2198,8 @@
       <c r="C18" s="2">
         <v>7</v>
       </c>
-      <c r="D18" s="2">
-        <v>7</v>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="E18" s="2">
         <v>28</v>
@@ -2185,11 +2221,11 @@
       <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="C19" s="2">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2">
-        <v>7</v>
+      <c r="C19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E19" s="2">
         <v>28</v>
@@ -2214,8 +2250,8 @@
       <c r="C20" s="2">
         <v>8</v>
       </c>
-      <c r="D20" s="2">
-        <v>8</v>
+      <c r="D20" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E20" s="2">
         <v>29</v>
@@ -2237,11 +2273,11 @@
       <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="C21" s="2">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2">
-        <v>8.5</v>
+      <c r="C21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="E21" s="2">
         <v>30</v>
@@ -2262,1211 +2298,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBEFC84-B3D8-FE4A-AFC9-8F9DD284FE98}">
-  <dimension ref="A1:I41"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="2">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>-2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="2">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-2</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="2">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-2</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="2">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>-2</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="2">
-        <v>15</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B7" s="2">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-1</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="2">
-        <v>17</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B8" s="2">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-1</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="2">
-        <v>17</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B9" s="2">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="2">
-        <v>19</v>
-      </c>
-      <c r="F9" s="2">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="2">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B11" s="2">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="2">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2">
-        <v>9</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B12" s="2">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2">
-        <v>21</v>
-      </c>
-      <c r="F12" s="2">
-        <v>13</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B13" s="2">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2">
-        <v>21</v>
-      </c>
-      <c r="F13" s="2">
-        <v>13</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B14" s="2">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2">
-        <v>23</v>
-      </c>
-      <c r="F14" s="2">
-        <v>16</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B15" s="2">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2">
-        <v>4</v>
-      </c>
-      <c r="D15" s="2">
-        <v>4</v>
-      </c>
-      <c r="E15" s="2">
-        <v>24</v>
-      </c>
-      <c r="F15" s="2">
-        <v>21</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B16" s="2">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>26</v>
-      </c>
-      <c r="F16" s="2">
-        <v>23</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B17" s="2">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2">
-        <v>6</v>
-      </c>
-      <c r="D17" s="2">
-        <v>6</v>
-      </c>
-      <c r="E17" s="2">
-        <v>27</v>
-      </c>
-      <c r="F17" s="2">
-        <v>27</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A18" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B18" s="2">
-        <v>17</v>
-      </c>
-      <c r="C18" s="2">
-        <v>7</v>
-      </c>
-      <c r="D18" s="2">
-        <v>7</v>
-      </c>
-      <c r="E18" s="2">
-        <v>28</v>
-      </c>
-      <c r="F18" s="2">
-        <v>28</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B19" s="2">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2">
-        <v>7</v>
-      </c>
-      <c r="E19" s="2">
-        <v>28</v>
-      </c>
-      <c r="F19" s="2">
-        <v>28</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A20" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B20" s="2">
-        <v>19</v>
-      </c>
-      <c r="C20" s="2">
-        <v>8</v>
-      </c>
-      <c r="D20" s="2">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2">
-        <v>29</v>
-      </c>
-      <c r="F20" s="2">
-        <v>30</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A21" s="1">
-        <v>1425</v>
-      </c>
-      <c r="B21" s="2">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="E21" s="2">
-        <v>30</v>
-      </c>
-      <c r="F21" s="2">
-        <v>32</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A22" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B22" s="7">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7">
-        <v>-2</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="7">
-        <v>15</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="7">
-        <v>0</v>
-      </c>
-      <c r="I22" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A23" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B23" s="7">
-        <v>2</v>
-      </c>
-      <c r="C23" s="7">
-        <v>-2</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="7">
-        <v>15</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="7">
-        <v>0</v>
-      </c>
-      <c r="I23" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A24" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B24" s="7">
-        <v>3</v>
-      </c>
-      <c r="C24" s="7">
-        <v>-2</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="7">
-        <v>15</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="7">
-        <v>0</v>
-      </c>
-      <c r="I24" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A25" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B25" s="7">
-        <v>4</v>
-      </c>
-      <c r="C25" s="7">
-        <v>-2</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="7">
-        <v>15</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="7">
-        <v>0</v>
-      </c>
-      <c r="I25" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A26" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B26" s="7">
-        <v>5</v>
-      </c>
-      <c r="C26" s="7">
-        <v>-2</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="7">
-        <v>15</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="7">
-        <v>0</v>
-      </c>
-      <c r="I26" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A27" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B27" s="7">
-        <v>6</v>
-      </c>
-      <c r="C27" s="7">
-        <v>-2</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="7">
-        <v>15</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="7">
-        <v>0</v>
-      </c>
-      <c r="I27" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A28" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B28" s="7">
-        <v>7</v>
-      </c>
-      <c r="C28" s="7">
-        <v>-2</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="7">
-        <v>15</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0</v>
-      </c>
-      <c r="I28" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A29" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B29" s="7">
-        <v>8</v>
-      </c>
-      <c r="C29" s="7">
-        <v>-1</v>
-      </c>
-      <c r="D29" s="7">
-        <v>-1</v>
-      </c>
-      <c r="E29" s="7">
-        <v>17</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A30" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B30" s="7">
-        <v>9</v>
-      </c>
-      <c r="C30" s="7">
-        <v>-1</v>
-      </c>
-      <c r="D30" s="7">
-        <v>-1</v>
-      </c>
-      <c r="E30" s="7">
-        <v>17</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A31" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B31" s="7">
-        <v>10</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="7">
-        <v>19</v>
-      </c>
-      <c r="F31" s="7">
-        <v>9</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A32" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B32" s="7">
-        <v>11</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="7">
-        <v>19</v>
-      </c>
-      <c r="F32" s="7">
-        <v>9</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A33" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B33" s="7">
-        <v>12</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="7">
-        <v>19</v>
-      </c>
-      <c r="F33" s="7">
-        <v>9</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A34" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B34" s="7">
-        <v>13</v>
-      </c>
-      <c r="C34" s="7">
-        <v>2</v>
-      </c>
-      <c r="D34" s="7">
-        <v>2</v>
-      </c>
-      <c r="E34" s="7">
-        <v>21</v>
-      </c>
-      <c r="F34" s="7">
-        <v>13</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A35" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B35" s="7">
-        <v>14</v>
-      </c>
-      <c r="C35" s="7">
-        <v>2</v>
-      </c>
-      <c r="D35" s="7">
-        <v>2</v>
-      </c>
-      <c r="E35" s="7">
-        <v>21</v>
-      </c>
-      <c r="F35" s="7">
-        <v>13</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A36" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B36" s="7">
-        <v>15</v>
-      </c>
-      <c r="C36" s="7">
-        <v>3</v>
-      </c>
-      <c r="D36" s="7">
-        <v>3</v>
-      </c>
-      <c r="E36" s="7">
-        <v>23</v>
-      </c>
-      <c r="F36" s="7">
-        <v>16</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A37" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B37" s="7">
-        <v>16</v>
-      </c>
-      <c r="C37" s="7">
-        <v>4</v>
-      </c>
-      <c r="D37" s="7">
-        <v>4</v>
-      </c>
-      <c r="E37" s="7">
-        <v>24</v>
-      </c>
-      <c r="F37" s="7">
-        <v>21</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A38" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B38" s="7">
-        <v>17</v>
-      </c>
-      <c r="C38" s="7">
-        <v>5</v>
-      </c>
-      <c r="D38" s="7">
-        <v>5</v>
-      </c>
-      <c r="E38" s="7">
-        <v>26</v>
-      </c>
-      <c r="F38" s="7">
-        <v>23</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I38" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A39" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B39" s="7">
-        <v>18</v>
-      </c>
-      <c r="C39" s="7">
-        <v>6</v>
-      </c>
-      <c r="D39" s="7">
-        <v>6</v>
-      </c>
-      <c r="E39" s="7">
-        <v>27</v>
-      </c>
-      <c r="F39" s="7">
-        <v>27</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I39" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A40" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B40" s="7">
-        <v>19</v>
-      </c>
-      <c r="C40" s="7">
-        <v>7</v>
-      </c>
-      <c r="D40" s="7">
-        <v>7</v>
-      </c>
-      <c r="E40" s="7">
-        <v>28</v>
-      </c>
-      <c r="F40" s="7">
-        <v>28</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40" s="7">
-        <v>1</v>
-      </c>
-      <c r="I40" s="8">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A41" s="6">
-        <v>1425</v>
-      </c>
-      <c r="B41" s="7">
-        <v>20</v>
-      </c>
-      <c r="C41" s="7">
-        <v>7</v>
-      </c>
-      <c r="D41" s="7">
-        <v>7</v>
-      </c>
-      <c r="E41" s="7">
-        <v>28</v>
-      </c>
-      <c r="F41" s="7">
-        <v>28</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" s="7">
-        <v>1</v>
-      </c>
-      <c r="I41" s="8">
-        <v>425</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3474,7 +2305,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3610,7 +2441,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="4">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>32</v>
@@ -3630,7 +2461,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="4">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>32</v>
@@ -3650,7 +2481,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>34</v>
@@ -3670,7 +2501,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="4">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>34</v>
@@ -3690,7 +2521,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="4">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>36</v>
@@ -3710,7 +2541,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="4">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>36</v>
@@ -3730,7 +2561,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="4">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>37</v>
@@ -3750,7 +2581,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="4">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>39</v>
@@ -3770,7 +2601,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="4">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>34</v>
@@ -3790,7 +2621,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="4">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>40</v>
@@ -3810,7 +2641,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="4">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>40</v>
@@ -3830,7 +2661,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="4">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>40</v>
@@ -3850,7 +2681,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="4">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>40</v>
@@ -3870,7 +2701,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="4">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>40</v>
@@ -3890,7 +2721,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="4">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>40</v>
@@ -4307,11 +3138,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E34554-567E-4640-BB10-BF8C510B0742}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -4499,7 +3330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B2EE7A-CE72-9144-B8A8-52A552CB2EEF}">
   <dimension ref="A1:J24"/>
   <sheetViews>
@@ -5020,4 +3851,1209 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBEFC84-B3D8-FE4A-AFC9-8F9DD284FE98}">
+  <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="2">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="2">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="2">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="2">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>21</v>
+      </c>
+      <c r="F13" s="2">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2">
+        <v>24</v>
+      </c>
+      <c r="F15" s="2">
+        <v>21</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>26</v>
+      </c>
+      <c r="F16" s="2">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2">
+        <v>27</v>
+      </c>
+      <c r="F17" s="2">
+        <v>27</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2">
+        <v>28</v>
+      </c>
+      <c r="F18" s="2">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>28</v>
+      </c>
+      <c r="F19" s="2">
+        <v>28</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
+        <v>1425</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="E21" s="2">
+        <v>30</v>
+      </c>
+      <c r="F21" s="2">
+        <v>32</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B22" s="7">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7">
+        <v>-2</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="7">
+        <v>15</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2</v>
+      </c>
+      <c r="C23" s="7">
+        <v>-2</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="7">
+        <v>15</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0</v>
+      </c>
+      <c r="I23" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B24" s="7">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7">
+        <v>-2</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="7">
+        <v>15</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0</v>
+      </c>
+      <c r="I24" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B25" s="7">
+        <v>4</v>
+      </c>
+      <c r="C25" s="7">
+        <v>-2</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="7">
+        <v>15</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0</v>
+      </c>
+      <c r="I25" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B26" s="7">
+        <v>5</v>
+      </c>
+      <c r="C26" s="7">
+        <v>-2</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="7">
+        <v>15</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0</v>
+      </c>
+      <c r="I26" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B27" s="7">
+        <v>6</v>
+      </c>
+      <c r="C27" s="7">
+        <v>-2</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="7">
+        <v>15</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="7">
+        <v>0</v>
+      </c>
+      <c r="I27" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B28" s="7">
+        <v>7</v>
+      </c>
+      <c r="C28" s="7">
+        <v>-2</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="7">
+        <v>15</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0</v>
+      </c>
+      <c r="I28" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B29" s="7">
+        <v>8</v>
+      </c>
+      <c r="C29" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E29" s="7">
+        <v>17</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B30" s="7">
+        <v>9</v>
+      </c>
+      <c r="C30" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D30" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="7">
+        <v>17</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B31" s="7">
+        <v>10</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="7">
+        <v>19</v>
+      </c>
+      <c r="F31" s="7">
+        <v>9</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B32" s="7">
+        <v>11</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="7">
+        <v>19</v>
+      </c>
+      <c r="F32" s="7">
+        <v>9</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B33" s="7">
+        <v>12</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="7">
+        <v>19</v>
+      </c>
+      <c r="F33" s="7">
+        <v>9</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B34" s="7">
+        <v>13</v>
+      </c>
+      <c r="C34" s="7">
+        <v>2</v>
+      </c>
+      <c r="D34" s="7">
+        <v>2</v>
+      </c>
+      <c r="E34" s="7">
+        <v>21</v>
+      </c>
+      <c r="F34" s="7">
+        <v>13</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B35" s="7">
+        <v>14</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2</v>
+      </c>
+      <c r="D35" s="7">
+        <v>2</v>
+      </c>
+      <c r="E35" s="7">
+        <v>21</v>
+      </c>
+      <c r="F35" s="7">
+        <v>13</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B36" s="7">
+        <v>15</v>
+      </c>
+      <c r="C36" s="7">
+        <v>3</v>
+      </c>
+      <c r="D36" s="7">
+        <v>3</v>
+      </c>
+      <c r="E36" s="7">
+        <v>23</v>
+      </c>
+      <c r="F36" s="7">
+        <v>16</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B37" s="7">
+        <v>16</v>
+      </c>
+      <c r="C37" s="7">
+        <v>4</v>
+      </c>
+      <c r="D37" s="7">
+        <v>4</v>
+      </c>
+      <c r="E37" s="7">
+        <v>24</v>
+      </c>
+      <c r="F37" s="7">
+        <v>21</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B38" s="7">
+        <v>17</v>
+      </c>
+      <c r="C38" s="7">
+        <v>5</v>
+      </c>
+      <c r="D38" s="7">
+        <v>5</v>
+      </c>
+      <c r="E38" s="7">
+        <v>26</v>
+      </c>
+      <c r="F38" s="7">
+        <v>23</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B39" s="7">
+        <v>18</v>
+      </c>
+      <c r="C39" s="7">
+        <v>6</v>
+      </c>
+      <c r="D39" s="7">
+        <v>6</v>
+      </c>
+      <c r="E39" s="7">
+        <v>27</v>
+      </c>
+      <c r="F39" s="7">
+        <v>27</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B40" s="7">
+        <v>19</v>
+      </c>
+      <c r="C40" s="7">
+        <v>7</v>
+      </c>
+      <c r="D40" s="7">
+        <v>7</v>
+      </c>
+      <c r="E40" s="7">
+        <v>28</v>
+      </c>
+      <c r="F40" s="7">
+        <v>28</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1</v>
+      </c>
+      <c r="I40" s="8">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" s="6">
+        <v>1425</v>
+      </c>
+      <c r="B41" s="7">
+        <v>20</v>
+      </c>
+      <c r="C41" s="7">
+        <v>7</v>
+      </c>
+      <c r="D41" s="7">
+        <v>7</v>
+      </c>
+      <c r="E41" s="7">
+        <v>28</v>
+      </c>
+      <c r="F41" s="7">
+        <v>28</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="7">
+        <v>1</v>
+      </c>
+      <c r="I41" s="8">
+        <v>425</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>